<commit_message>
extensão do ano máximo até 2060
</commit_message>
<xml_diff>
--- a/inst/dados_premissas/2022/crescimento_mercado.xlsx
+++ b/inst/dados_premissas/2022/crescimento_mercado.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arquivos Locais\projetos\epe4md-git3\inst\dados_premissas\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6855F56-BB99-4622-9BDC-A99519C6EA08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37154752-EF32-42A2-920E-A17831CB9195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -353,15 +353,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="10" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -711,6 +711,86 @@
         <v>0.03</v>
       </c>
     </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>2051</v>
+      </c>
+      <c r="B43">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>2052</v>
+      </c>
+      <c r="B44">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>2053</v>
+      </c>
+      <c r="B45">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>2054</v>
+      </c>
+      <c r="B46">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>2055</v>
+      </c>
+      <c r="B47">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>2056</v>
+      </c>
+      <c r="B48">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>2057</v>
+      </c>
+      <c r="B49">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>2058</v>
+      </c>
+      <c r="B50">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>2059</v>
+      </c>
+      <c r="B51">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>2060</v>
+      </c>
+      <c r="B52">
+        <v>0.03</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização de planilhas para a 2ªRevisão Qaudrimestral 2023-2027.
</commit_message>
<xml_diff>
--- a/inst/dados_premissas/2022/crescimento_mercado.xlsx
+++ b/inst/dados_premissas/2022/crescimento_mercado.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arquivos Locais\projetos\epe4md-git3\inst\dados_premissas\2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Geracao Distribuida\PDE\PDE2033_2RQ\dados_premissas\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37154752-EF32-42A2-920E-A17831CB9195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC72417-04F8-4D82-BCD4-68A50ADB9CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -353,15 +353,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -474,7 +474,7 @@
         <v>2022</v>
       </c>
       <c r="B14">
-        <v>2.9000000000000001E-2</v>
+        <v>0.03</v>
       </c>
       <c r="D14" s="2"/>
     </row>
@@ -483,7 +483,7 @@
         <v>2023</v>
       </c>
       <c r="B15">
-        <v>0.01</v>
+        <v>2.3E-2</v>
       </c>
       <c r="D15" s="2"/>
     </row>
@@ -501,7 +501,7 @@
         <v>2025</v>
       </c>
       <c r="B17">
-        <v>0.02</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="D17" s="2"/>
     </row>
@@ -708,86 +708,6 @@
         <v>2050</v>
       </c>
       <c r="B42">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>2051</v>
-      </c>
-      <c r="B43">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>2052</v>
-      </c>
-      <c r="B44">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>2053</v>
-      </c>
-      <c r="B45">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>2054</v>
-      </c>
-      <c r="B46">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>2055</v>
-      </c>
-      <c r="B47">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>2056</v>
-      </c>
-      <c r="B48">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>2057</v>
-      </c>
-      <c r="B49">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>2058</v>
-      </c>
-      <c r="B50">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>2059</v>
-      </c>
-      <c r="B51">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>2060</v>
-      </c>
-      <c r="B52">
         <v>0.03</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização de planilhas para o PLAN2024-2028.
</commit_message>
<xml_diff>
--- a/inst/dados_premissas/2022/crescimento_mercado.xlsx
+++ b/inst/dados_premissas/2022/crescimento_mercado.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Geracao Distribuida\PDE\PDE2033_2RQ\dados_premissas\2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Geracao Distribuida\PDE\PDE2034_2RQ\dados_premissas\2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC72417-04F8-4D82-BCD4-68A50ADB9CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4860C4-4088-4D90-A06B-8F51FE4F795A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -37,14 +48,27 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -66,16 +90,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -353,18 +381,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="9.9499999999999993" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -372,7 +400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="9.9499999999999993" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2010</v>
       </c>
@@ -380,7 +408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="9.9499999999999993" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2011</v>
       </c>
@@ -388,7 +416,7 @@
         <v>3.9699999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="9.9499999999999993" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2012</v>
       </c>
@@ -396,7 +424,7 @@
         <v>1.9199999999999998E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="9.9499999999999993" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2013</v>
       </c>
@@ -404,7 +432,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="9.9499999999999993" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2014</v>
       </c>
@@ -412,7 +440,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="9.9499999999999993" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2015</v>
       </c>
@@ -420,7 +448,7 @@
         <v>-3.7699999999999997E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="9.9499999999999993" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2016</v>
       </c>
@@ -428,7 +456,7 @@
         <v>-3.5900000000000001E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="9.9499999999999993" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2017</v>
       </c>
@@ -436,7 +464,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="9.9499999999999993" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2018</v>
       </c>
@@ -444,7 +472,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="9.9499999999999993" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2019</v>
       </c>
@@ -452,7 +480,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="9.9499999999999993" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2020</v>
       </c>
@@ -460,7 +488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="9.9499999999999993" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2021</v>
       </c>
@@ -469,169 +497,197 @@
       </c>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2022</v>
       </c>
       <c r="B14">
-        <v>0.03</v>
-      </c>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2023</v>
       </c>
       <c r="B15">
-        <v>2.3E-2</v>
-      </c>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3.2000000000000028E-2</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2024</v>
       </c>
       <c r="B16">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.0000000000000018E-2</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2025</v>
       </c>
       <c r="B17">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.200000000000002E-2</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2026</v>
       </c>
       <c r="B18">
-        <v>2.3E-2</v>
-      </c>
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.2999999999999909E-2</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2027</v>
       </c>
       <c r="B19">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.4999999999999911E-2</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2028</v>
       </c>
       <c r="B20">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.9999999999999805E-2</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2029</v>
       </c>
       <c r="B21">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3.0000000000000249E-2</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2030</v>
       </c>
       <c r="B22">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3.0000000000000249E-2</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2031</v>
       </c>
       <c r="B23">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="4"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2032</v>
       </c>
       <c r="B24">
-        <v>2.8000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.9999999999999805E-2</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="4"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2033</v>
       </c>
       <c r="B25">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3.0000000000000249E-2</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2034</v>
       </c>
       <c r="B26">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2035</v>
       </c>
       <c r="B27">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.9999999999999805E-2</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2036</v>
       </c>
       <c r="B28">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3.0000000000000249E-2</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2037</v>
       </c>
       <c r="B29">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2038</v>
       </c>
       <c r="B30">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+        <v>2.9999999999999805E-2</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2039</v>
       </c>
       <c r="B31">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2040</v>
       </c>
       <c r="B32">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+        <v>3.0000000000000027E-2</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:2" ht="9.9499999999999993" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2041</v>
       </c>
@@ -639,7 +695,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" ht="9.9499999999999993" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2042</v>
       </c>
@@ -647,7 +703,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" ht="9.9499999999999993" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2043</v>
       </c>
@@ -655,7 +711,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" ht="9.9499999999999993" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2044</v>
       </c>
@@ -663,7 +719,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" ht="9.9499999999999993" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2045</v>
       </c>
@@ -671,7 +727,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" ht="9.9499999999999993" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2046</v>
       </c>
@@ -679,7 +735,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" ht="9.9499999999999993" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2047</v>
       </c>
@@ -687,7 +743,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" ht="9.9499999999999993" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2048</v>
       </c>
@@ -695,7 +751,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" ht="9.9499999999999993" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2049</v>
       </c>
@@ -703,7 +759,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" ht="9.9499999999999993" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2050</v>
       </c>

</xml_diff>